<commit_message>
Format Changes to Table
</commit_message>
<xml_diff>
--- a/P3TOME_MAIN_TABLE.xlsx
+++ b/P3TOME_MAIN_TABLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8568\Documents\GitHub\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajf/Documents/GitHub/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C19F6A-26E0-4253-9CA0-2A7949B4EAF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A168B60-E830-9549-9E9E-23B18C3D8073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BF91EB68-8200-D04C-ACEA-7728D8B81486}"/>
+    <workbookView xWindow="-4120" yWindow="-18520" windowWidth="31120" windowHeight="19860" xr2:uid="{BF91EB68-8200-D04C-ACEA-7728D8B81486}"/>
   </bookViews>
   <sheets>
     <sheet name="P3Tome" sheetId="1" r:id="rId1"/>
@@ -533,7 +533,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -825,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -888,9 +888,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -913,6 +910,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -945,35 +966,58 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="9" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1285,74 +1329,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470AE0E9-15FB-9B45-982A-B5C4188457EE}">
   <dimension ref="A1:BD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.296875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="16" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.796875" style="9"/>
-    <col min="4" max="4" width="62.296875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="60.296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.296875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="62" style="9" customWidth="1"/>
+    <col min="5" max="5" width="60.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" style="9" customWidth="1"/>
     <col min="7" max="7" width="38" style="9" customWidth="1"/>
-    <col min="8" max="8" width="14.796875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" style="9" customWidth="1"/>
     <col min="9" max="9" width="18.5" style="9" customWidth="1"/>
-    <col min="10" max="10" width="14.69921875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="9" customWidth="1"/>
     <col min="11" max="11" width="12" style="9" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="9" customWidth="1"/>
-    <col min="13" max="13" width="16.796875" style="9" customWidth="1"/>
-    <col min="14" max="14" width="14.296875" style="9" customWidth="1"/>
-    <col min="15" max="15" width="10.796875" style="9"/>
-    <col min="16" max="16" width="31.69921875" style="9" customWidth="1"/>
-    <col min="17" max="17" width="33.796875" style="9" customWidth="1"/>
-    <col min="18" max="18" width="24.296875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="9"/>
+    <col min="16" max="16" width="31.6640625" style="9" customWidth="1"/>
+    <col min="17" max="17" width="33.83203125" style="9" customWidth="1"/>
+    <col min="18" max="18" width="24.33203125" style="9" customWidth="1"/>
     <col min="19" max="19" width="13" style="9" customWidth="1"/>
     <col min="20" max="20" width="26.5" style="9" customWidth="1"/>
-    <col min="21" max="21" width="28.69921875" style="9" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" style="9" customWidth="1"/>
     <col min="22" max="22" width="28" style="9" customWidth="1"/>
-    <col min="23" max="23" width="28.296875" style="9" customWidth="1"/>
-    <col min="24" max="24" width="24.796875" style="9" customWidth="1"/>
-    <col min="25" max="27" width="23.19921875" style="9" customWidth="1"/>
+    <col min="23" max="23" width="28.33203125" style="9" customWidth="1"/>
+    <col min="24" max="24" width="24.83203125" style="9" customWidth="1"/>
+    <col min="25" max="27" width="23.1640625" style="9" customWidth="1"/>
     <col min="28" max="28" width="35.5" style="9" customWidth="1"/>
     <col min="29" max="29" width="19.5" style="9" customWidth="1"/>
-    <col min="30" max="30" width="19.69921875" style="9" customWidth="1"/>
-    <col min="31" max="31" width="44.69921875" style="9" customWidth="1"/>
-    <col min="32" max="32" width="35.796875" style="9" customWidth="1"/>
-    <col min="33" max="33" width="40.19921875" style="9" customWidth="1"/>
+    <col min="30" max="30" width="19.6640625" style="9" customWidth="1"/>
+    <col min="31" max="31" width="44.6640625" style="9" customWidth="1"/>
+    <col min="32" max="32" width="35.83203125" style="9" customWidth="1"/>
+    <col min="33" max="33" width="40.1640625" style="9" customWidth="1"/>
     <col min="34" max="34" width="29" style="9" customWidth="1"/>
     <col min="35" max="35" width="49.5" style="9" customWidth="1"/>
-    <col min="36" max="36" width="51.796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="53.8984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="51.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="53.83203125" style="9" bestFit="1" customWidth="1"/>
     <col min="38" max="41" width="54.5" style="9" customWidth="1"/>
-    <col min="42" max="42" width="42.59765625" style="9" customWidth="1"/>
-    <col min="43" max="43" width="32.296875" style="9" customWidth="1"/>
+    <col min="42" max="42" width="42.6640625" style="9" customWidth="1"/>
+    <col min="43" max="43" width="32.33203125" style="9" customWidth="1"/>
     <col min="44" max="44" width="54.5" style="9" customWidth="1"/>
-    <col min="45" max="45" width="12.69921875" style="9" customWidth="1"/>
+    <col min="45" max="45" width="12.6640625" style="9" customWidth="1"/>
     <col min="46" max="46" width="19.5" style="9" customWidth="1"/>
-    <col min="47" max="47" width="20.296875" style="9" customWidth="1"/>
+    <col min="47" max="47" width="20.33203125" style="9" customWidth="1"/>
     <col min="48" max="48" width="22.5" style="9" customWidth="1"/>
-    <col min="49" max="49" width="10.796875" style="9"/>
-    <col min="50" max="50" width="13.19921875" style="9" customWidth="1"/>
-    <col min="51" max="51" width="10.796875" style="9"/>
-    <col min="52" max="52" width="12.59765625" style="9" customWidth="1"/>
-    <col min="53" max="16384" width="10.796875" style="9"/>
+    <col min="49" max="49" width="10.83203125" style="9"/>
+    <col min="50" max="50" width="13.1640625" style="9" customWidth="1"/>
+    <col min="51" max="51" width="10.83203125" style="9"/>
+    <col min="52" max="52" width="12.6640625" style="9" customWidth="1"/>
+    <col min="53" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="103.95" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:56" ht="104" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="35"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
@@ -1419,77 +1463,77 @@
       <c r="BC1" s="11"/>
       <c r="BD1" s="11"/>
     </row>
-    <row r="2" spans="1:56">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="40" t="s">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="39" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="46"/>
+      <c r="J2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="42" t="s">
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="38" t="s">
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="38"/>
-      <c r="AC2" s="38"/>
-      <c r="AD2" s="38"/>
-      <c r="AE2" s="38"/>
-      <c r="AF2" s="38"/>
-      <c r="AG2" s="38"/>
-      <c r="AH2" s="38"/>
-      <c r="AI2" s="38"/>
-      <c r="AJ2" s="38"/>
-      <c r="AK2" s="38"/>
-      <c r="AL2" s="38"/>
-      <c r="AM2" s="26"/>
-      <c r="AN2" s="26"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="26"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="37" t="s">
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="45"/>
+      <c r="AC2" s="45"/>
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="45"/>
+      <c r="AL2" s="45"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="25"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="AT2" s="37"/>
-      <c r="AU2" s="37"/>
-      <c r="AV2" s="37"/>
-      <c r="AW2" s="37"/>
-      <c r="AX2" s="37"/>
-      <c r="AY2" s="37"/>
-      <c r="AZ2" s="37"/>
-      <c r="BA2" s="37"/>
-      <c r="BB2" s="37"/>
-      <c r="BC2" s="37"/>
-      <c r="BD2" s="37"/>
-    </row>
-    <row r="3" spans="1:56" ht="72">
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
+      <c r="AW2" s="44"/>
+      <c r="AX2" s="44"/>
+      <c r="AY2" s="44"/>
+      <c r="AZ2" s="44"/>
+      <c r="BA2" s="44"/>
+      <c r="BB2" s="44"/>
+      <c r="BC2" s="44"/>
+      <c r="BD2" s="44"/>
+    </row>
+    <row r="3" spans="1:56" ht="100" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>99</v>
       </c>
@@ -1529,7 +1573,7 @@
       <c r="M3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="20" t="s">
         <v>34</v>
       </c>
       <c r="O3" s="20" t="s">
@@ -1560,13 +1604,13 @@
         <v>95</v>
       </c>
       <c r="X3" s="20"/>
-      <c r="Y3" s="31" t="s">
+      <c r="Y3" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="Z3" s="31" t="s">
+      <c r="Z3" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="AA3" s="31" t="s">
+      <c r="AA3" s="30" t="s">
         <v>127</v>
       </c>
       <c r="AB3" s="20" t="s">
@@ -1599,49 +1643,49 @@
       <c r="AK3" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="AL3" s="24" t="s">
+      <c r="AL3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="AM3" s="24" t="s">
+      <c r="AM3" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="AN3" s="28" t="s">
+      <c r="AN3" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="AO3" s="28" t="s">
+      <c r="AO3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="AP3" s="28" t="s">
+      <c r="AP3" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="AQ3" s="28" t="s">
+      <c r="AQ3" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="AR3" s="28" t="s">
+      <c r="AR3" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="AS3" s="27" t="s">
+      <c r="AS3" s="26" t="s">
         <v>101</v>
       </c>
       <c r="AT3" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="AU3" s="27" t="s">
+      <c r="AU3" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="AV3" s="27" t="s">
+      <c r="AV3" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="AW3" s="27" t="s">
+      <c r="AW3" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="AX3" s="27" t="s">
+      <c r="AX3" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="AY3" s="27" t="s">
+      <c r="AY3" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="AZ3" s="27" t="s">
+      <c r="AZ3" s="26" t="s">
         <v>134</v>
       </c>
       <c r="BA3" s="21"/>
@@ -1649,7 +1693,7 @@
       <c r="BC3" s="21"/>
       <c r="BD3" s="21"/>
     </row>
-    <row r="4" spans="1:56">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>52</v>
       </c>
@@ -1694,7 +1738,7 @@
       <c r="P4" s="22">
         <v>0</v>
       </c>
-      <c r="Q4" s="30">
+      <c r="Q4" s="29">
         <v>0</v>
       </c>
       <c r="R4" s="10">
@@ -1805,7 +1849,7 @@
       <c r="BC4" s="10"/>
       <c r="BD4" s="10"/>
     </row>
-    <row r="5" spans="1:56">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>53</v>
       </c>
@@ -1850,7 +1894,7 @@
       <c r="P5" s="22">
         <v>0</v>
       </c>
-      <c r="Q5" s="30">
+      <c r="Q5" s="29">
         <v>0</v>
       </c>
       <c r="R5" s="10">
@@ -1961,7 +2005,7 @@
       <c r="BC5" s="10"/>
       <c r="BD5" s="10"/>
     </row>
-    <row r="6" spans="1:56">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>54</v>
       </c>
@@ -2006,7 +2050,7 @@
       <c r="P6" s="22">
         <v>0</v>
       </c>
-      <c r="Q6" s="30">
+      <c r="Q6" s="29">
         <v>0</v>
       </c>
       <c r="R6" s="10">
@@ -2117,7 +2161,7 @@
       <c r="BC6" s="10"/>
       <c r="BD6" s="10"/>
     </row>
-    <row r="7" spans="1:56">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>55</v>
       </c>
@@ -2162,7 +2206,7 @@
       <c r="P7" s="22">
         <v>0</v>
       </c>
-      <c r="Q7" s="30">
+      <c r="Q7" s="29">
         <v>0</v>
       </c>
       <c r="R7" s="10">
@@ -2273,7 +2317,7 @@
       <c r="BC7" s="10"/>
       <c r="BD7" s="10"/>
     </row>
-    <row r="8" spans="1:56">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>56</v>
       </c>
@@ -2318,7 +2362,7 @@
       <c r="P8" s="22">
         <v>0</v>
       </c>
-      <c r="Q8" s="30">
+      <c r="Q8" s="29">
         <v>0</v>
       </c>
       <c r="R8" s="10">
@@ -2429,7 +2473,7 @@
       <c r="BC8" s="10"/>
       <c r="BD8" s="10"/>
     </row>
-    <row r="9" spans="1:56">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>57</v>
       </c>
@@ -2474,7 +2518,7 @@
       <c r="P9" s="22">
         <v>0</v>
       </c>
-      <c r="Q9" s="30">
+      <c r="Q9" s="29">
         <v>0</v>
       </c>
       <c r="R9" s="10">
@@ -2585,7 +2629,7 @@
       <c r="BC9" s="10"/>
       <c r="BD9" s="10"/>
     </row>
-    <row r="10" spans="1:56">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>58</v>
       </c>
@@ -2630,7 +2674,7 @@
       <c r="P10" s="22">
         <v>0</v>
       </c>
-      <c r="Q10" s="30">
+      <c r="Q10" s="29">
         <v>0</v>
       </c>
       <c r="R10" s="10">
@@ -2741,7 +2785,7 @@
       <c r="BC10" s="10"/>
       <c r="BD10" s="10"/>
     </row>
-    <row r="11" spans="1:56">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>59</v>
       </c>
@@ -2786,7 +2830,7 @@
       <c r="P11" s="22">
         <v>0</v>
       </c>
-      <c r="Q11" s="30">
+      <c r="Q11" s="29">
         <v>0</v>
       </c>
       <c r="R11" s="10">
@@ -2897,11 +2941,11 @@
       <c r="BC11" s="10"/>
       <c r="BD11" s="10"/>
     </row>
-    <row r="12" spans="1:56">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="8">
@@ -3033,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:56">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>61</v>
       </c>
@@ -3181,7 +3225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:56">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>62</v>
       </c>
@@ -3329,7 +3373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:56">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>63</v>
       </c>
@@ -3377,7 +3421,7 @@
       <c r="Q15" s="9">
         <v>1</v>
       </c>
-      <c r="R15" s="29">
+      <c r="R15" s="28">
         <v>1</v>
       </c>
       <c r="S15" s="9">
@@ -3389,10 +3433,10 @@
       <c r="U15" s="9">
         <v>0</v>
       </c>
-      <c r="V15" s="29">
-        <v>0</v>
-      </c>
-      <c r="W15" s="29">
+      <c r="V15" s="28">
+        <v>0</v>
+      </c>
+      <c r="W15" s="28">
         <v>1</v>
       </c>
       <c r="Y15" s="9">
@@ -3480,7 +3524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:56">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>64</v>
       </c>
@@ -3528,7 +3572,7 @@
       <c r="Q16" s="9">
         <v>1</v>
       </c>
-      <c r="R16" s="29">
+      <c r="R16" s="28">
         <v>1</v>
       </c>
       <c r="S16" s="9">
@@ -3540,10 +3584,10 @@
       <c r="U16" s="9">
         <v>0</v>
       </c>
-      <c r="V16" s="29">
-        <v>0</v>
-      </c>
-      <c r="W16" s="29">
+      <c r="V16" s="28">
+        <v>0</v>
+      </c>
+      <c r="W16" s="28">
         <v>1</v>
       </c>
       <c r="Y16" s="9">
@@ -3631,7 +3675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:52">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>65</v>
       </c>
@@ -3782,155 +3826,155 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:52" s="46" customFormat="1">
-      <c r="A18" s="43" t="s">
+    <row r="18" spans="1:52" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45">
+      <c r="B18" s="33"/>
+      <c r="C18" s="34">
         <v>15</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="H18" s="47">
-        <v>1</v>
-      </c>
-      <c r="I18" s="47"/>
-      <c r="J18" s="46">
-        <v>1</v>
-      </c>
-      <c r="K18" s="46">
-        <v>0</v>
-      </c>
-      <c r="L18" s="46">
-        <v>1</v>
-      </c>
-      <c r="M18" s="46">
-        <v>1</v>
-      </c>
-      <c r="N18" s="46">
-        <v>1</v>
-      </c>
-      <c r="O18" s="46">
-        <v>0</v>
-      </c>
-      <c r="P18" s="46">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="46">
-        <v>1</v>
-      </c>
-      <c r="R18" s="46">
-        <v>0</v>
-      </c>
-      <c r="S18" s="48">
-        <v>0</v>
-      </c>
-      <c r="T18" s="48">
-        <v>0</v>
-      </c>
-      <c r="U18" s="48">
-        <v>0</v>
-      </c>
-      <c r="V18" s="48">
-        <v>0</v>
-      </c>
-      <c r="W18" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="46">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AH18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AI18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AK18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AL18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AM18" s="46">
-        <v>1</v>
-      </c>
-      <c r="AN18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AO18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AP18" s="49">
-        <v>0</v>
-      </c>
-      <c r="AQ18" s="49">
-        <v>0</v>
-      </c>
-      <c r="AR18" s="49">
-        <v>0</v>
-      </c>
-      <c r="AS18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AT18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AU18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AV18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AW18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AX18" s="46">
-        <v>1</v>
-      </c>
-      <c r="AY18" s="46">
-        <v>0</v>
-      </c>
-      <c r="AZ18" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:52">
+      <c r="H18" s="36">
+        <v>1</v>
+      </c>
+      <c r="I18" s="36"/>
+      <c r="J18" s="35">
+        <v>1</v>
+      </c>
+      <c r="K18" s="35">
+        <v>0</v>
+      </c>
+      <c r="L18" s="35">
+        <v>1</v>
+      </c>
+      <c r="M18" s="35">
+        <v>1</v>
+      </c>
+      <c r="N18" s="35">
+        <v>1</v>
+      </c>
+      <c r="O18" s="35">
+        <v>0</v>
+      </c>
+      <c r="P18" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="35">
+        <v>1</v>
+      </c>
+      <c r="R18" s="35">
+        <v>0</v>
+      </c>
+      <c r="S18" s="37">
+        <v>0</v>
+      </c>
+      <c r="T18" s="37">
+        <v>0</v>
+      </c>
+      <c r="U18" s="37">
+        <v>0</v>
+      </c>
+      <c r="V18" s="37">
+        <v>0</v>
+      </c>
+      <c r="W18" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="35">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AO18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="38">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="38">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="38">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AV18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AW18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AX18" s="35">
+        <v>1</v>
+      </c>
+      <c r="AY18" s="35">
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>67</v>
       </c>
@@ -4081,7 +4125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:52">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>68</v>
       </c>
@@ -4232,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:52">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>69</v>
       </c>
@@ -4383,7 +4427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:52">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>70</v>
       </c>
@@ -4531,7 +4575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:52">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>71</v>
       </c>
@@ -4547,10 +4591,10 @@
       <c r="F23" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H23" s="50">
-        <v>1</v>
-      </c>
-      <c r="I23" s="50"/>
+      <c r="H23" s="39">
+        <v>1</v>
+      </c>
+      <c r="I23" s="39"/>
       <c r="J23" s="9">
         <v>1</v>
       </c>
@@ -4678,52 +4722,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:52">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:52">
+    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:52">
+    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:52">
+    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:52">
+    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:52">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:52">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:52">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:52">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>81</v>
       </c>
@@ -4739,6 +4783,11 @@
     <mergeCell ref="J2:R2"/>
     <mergeCell ref="S2:X2"/>
   </mergeCells>
+  <conditionalFormatting sqref="Y4:AR23">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",Y4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
@@ -4755,17 +4804,17 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="23.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.19921875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="97.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32.69921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="54.5" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="10.796875" style="2"/>
+    <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" thickBot="1">
+    <row r="1" spans="1:5" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>98</v>
       </c>
@@ -4782,7 +4831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>17</v>
@@ -4797,7 +4846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -4806,7 +4855,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>15</v>
@@ -4815,7 +4864,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -4824,7 +4873,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -4833,7 +4882,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>16</v>
@@ -4842,7 +4891,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -4851,7 +4900,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>22</v>
@@ -4860,7 +4909,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -4869,7 +4918,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>26</v>
@@ -4878,7 +4927,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>97</v>
@@ -4887,73 +4936,73 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>

</xml_diff>